<commit_message>
almost finished group server
</commit_message>
<xml_diff>
--- a/microservice/serverURL.xlsx
+++ b/microservice/serverURL.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sean/Desktop/Stevens/690 software studio/SSW690Project/microservice/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AEA86C9A-1083-1B4F-BCB0-D4DFB448B71B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{562978A8-7D39-FB40-9304-7527BE6CF260}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14520" yWindow="0" windowWidth="14280" windowHeight="18000" xr2:uid="{CCCD09A4-18C6-E64F-BDB2-A2C4C6A74B84}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{CCCD09A4-18C6-E64F-BDB2-A2C4C6A74B84}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="44">
   <si>
     <t>group</t>
   </si>
@@ -39,9 +39,6 @@
     <t>getGroupName</t>
   </si>
   <si>
-    <t>8084/group/getGroupName/{groupId}</t>
-  </si>
-  <si>
     <t>String groupName</t>
   </si>
   <si>
@@ -60,15 +57,9 @@
     <t>createGroup</t>
   </si>
   <si>
-    <t>boolean</t>
-  </si>
-  <si>
     <t>getGroup</t>
   </si>
   <si>
-    <t>8084/group/getGroup/{groupId}</t>
-  </si>
-  <si>
     <t>Group group</t>
   </si>
   <si>
@@ -90,9 +81,6 @@
     <t>getTotalCheckoutState</t>
   </si>
   <si>
-    <t>8084/group/getTotalCheckoutState/{groupId}</t>
-  </si>
-  <si>
     <t>getUserCheckoutComfirm</t>
   </si>
   <si>
@@ -108,25 +96,73 @@
     <t>T</t>
   </si>
   <si>
-    <t>8084/group/createGroup/{groupName}_{userList}</t>
-  </si>
-  <si>
-    <t>8084/group/addMemberToGroup/{groupId}_{userList}</t>
-  </si>
-  <si>
-    <t>8084/group/getIndivitualTotalBalance/{groupId}_{userId}</t>
-  </si>
-  <si>
-    <t>8084/group/checkout/{groupId}_{userId}</t>
-  </si>
-  <si>
-    <t>8084/group/checkoutComfirm/{groupId}_{userId}_{state}</t>
-  </si>
-  <si>
-    <t>8084/group/getUserCheckoutComfirm/{groupId}_{userId}</t>
-  </si>
-  <si>
     <t>float totalBalance</t>
+  </si>
+  <si>
+    <t>Request</t>
+  </si>
+  <si>
+    <t>get</t>
+  </si>
+  <si>
+    <t>post</t>
+  </si>
+  <si>
+    <t>8084/group/</t>
+  </si>
+  <si>
+    <t>8084/group/{groupId}</t>
+  </si>
+  <si>
+    <t>8084/group/name/{groupId}</t>
+  </si>
+  <si>
+    <t>8084/group/users</t>
+  </si>
+  <si>
+    <t>8084/group/checkout/{groupId}</t>
+  </si>
+  <si>
+    <t>input body</t>
+  </si>
+  <si>
+    <t>String groupName, int[] usersList</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>int[] usersList, int groupId</t>
+  </si>
+  <si>
+    <t>8084/group/checkout/{groupId}/{userId}</t>
+  </si>
+  <si>
+    <t>8084/group/balance/{groupId}/{userId}</t>
+  </si>
+  <si>
+    <t>cancelCheckoutComfirm</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>8084/group/checkout/cancel/{groupId}/{userId}</t>
+  </si>
+  <si>
+    <t>getUserCancelCheckout</t>
+  </si>
+  <si>
+    <t>8084/group/checkout/cancel/{groupId}</t>
+  </si>
+  <si>
+    <t>int userId</t>
+  </si>
+  <si>
+    <t>TF</t>
+  </si>
+  <si>
+    <t>TP</t>
   </si>
 </sst>
 </file>
@@ -478,37 +514,43 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{624D0BFE-F7B1-024F-9FFD-32EB15BA65EB}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="22.33203125" customWidth="1"/>
-    <col min="3" max="3" width="49.83203125" customWidth="1"/>
-    <col min="4" max="4" width="21.5" customWidth="1"/>
+    <col min="2" max="3" width="22.33203125" customWidth="1"/>
+    <col min="4" max="5" width="49.83203125" customWidth="1"/>
+    <col min="6" max="6" width="21.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -516,107 +558,189 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>8</v>
       </c>
       <c r="C3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" t="s">
         <v>25</v>
       </c>
-      <c r="D3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="E4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B5" t="s">
+      <c r="D5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
         <v>10</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" t="s">
+        <v>35</v>
+      </c>
+      <c r="F6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
         <v>11</v>
       </c>
-      <c r="D5" t="s">
+      <c r="C7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" t="s">
         <v>12</v>
       </c>
-      <c r="E5" t="s">
+      <c r="G7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" t="s">
+        <v>29</v>
+      </c>
+      <c r="F8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" t="s">
-        <v>27</v>
-      </c>
-      <c r="D6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" t="s">
-        <v>28</v>
-      </c>
-      <c r="D7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B8" t="s">
+      <c r="D9" t="s">
+        <v>34</v>
+      </c>
+      <c r="F9" t="s">
+        <v>32</v>
+      </c>
+      <c r="G9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" t="s">
+        <v>40</v>
+      </c>
+      <c r="F10" t="s">
+        <v>41</v>
+      </c>
+      <c r="G10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" t="s">
+        <v>38</v>
+      </c>
+      <c r="F11" t="s">
+        <v>32</v>
+      </c>
+      <c r="G11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
         <v>16</v>
       </c>
-      <c r="C8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="C12" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" t="s">
+        <v>34</v>
+      </c>
+      <c r="F12" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B10" t="s">
+      <c r="G12" t="s">
         <v>20</v>
-      </c>
-      <c r="C10" t="s">
-        <v>30</v>
-      </c>
-      <c r="D10" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated group server, and finished bill server
</commit_message>
<xml_diff>
--- a/microservice/serverURL.xlsx
+++ b/microservice/serverURL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sean/Desktop/Stevens/690 software studio/SSW690Project/microservice/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{562978A8-7D39-FB40-9304-7527BE6CF260}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8BB7109-6C13-5E4C-B45C-CB54255159DC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{CCCD09A4-18C6-E64F-BDB2-A2C4C6A74B84}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="64">
   <si>
     <t>group</t>
   </si>
@@ -162,14 +162,74 @@
     <t>TF</t>
   </si>
   <si>
-    <t>TP</t>
+    <t>bill</t>
+  </si>
+  <si>
+    <t>getBill</t>
+  </si>
+  <si>
+    <t>getBillGeneral</t>
+  </si>
+  <si>
+    <t>createBill</t>
+  </si>
+  <si>
+    <t>billAddComfirm</t>
+  </si>
+  <si>
+    <t>getTotalAddState</t>
+  </si>
+  <si>
+    <t>cancelAddComfirm</t>
+  </si>
+  <si>
+    <t>getUserAddComfirm</t>
+  </si>
+  <si>
+    <t>getUserCancelAdd</t>
+  </si>
+  <si>
+    <t>8085/bill/general/{billId}</t>
+  </si>
+  <si>
+    <t>8085/bill/{billId}</t>
+  </si>
+  <si>
+    <t>8085/bill</t>
+  </si>
+  <si>
+    <t>8085/bill/add/{billId}</t>
+  </si>
+  <si>
+    <t>8085/bill/add/{billId}/{userId}</t>
+  </si>
+  <si>
+    <t>transfer</t>
+  </si>
+  <si>
+    <t>bill state chage</t>
+  </si>
+  <si>
+    <t>bill state</t>
+  </si>
+  <si>
+    <t>delete transfer</t>
+  </si>
+  <si>
+    <t>how to deal the bill been deleted?</t>
+  </si>
+  <si>
+    <t>8085/bill/cancel/{billId}/{userId}</t>
+  </si>
+  <si>
+    <t>8085/bill/cancel/{billId}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -177,16 +237,35 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -194,12 +273,87 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -514,10 +668,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{624D0BFE-F7B1-024F-9FFD-32EB15BA65EB}">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:I28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -527,223 +681,468 @@
     <col min="6" max="6" width="21.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="F2" t="s">
+      <c r="E2" s="2"/>
+      <c r="F2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B3" t="s">
+      <c r="G2" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="4"/>
+      <c r="B3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F3" t="s">
+      <c r="E3" s="2"/>
+      <c r="F3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B4" t="s">
+      <c r="G3" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="4"/>
+      <c r="B4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="G4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B5" t="s">
+      <c r="G4" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="4"/>
+      <c r="B5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="G5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B6" t="s">
+      <c r="G5" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="4"/>
+      <c r="B6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="F6" t="s">
+      <c r="E6" s="2"/>
+      <c r="F6" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B7" t="s">
+      <c r="G6" s="2"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="4"/>
+      <c r="B7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="H7" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="I7" s="11" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="4"/>
+      <c r="B8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C8" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D8" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F7" t="s">
+      <c r="E8" s="2"/>
+      <c r="F8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G8" s="2" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" t="s">
+      <c r="H8" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="I8" s="11" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="4"/>
+      <c r="B9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D8" t="s">
-        <v>29</v>
-      </c>
-      <c r="F8" t="s">
-        <v>14</v>
-      </c>
-      <c r="G8" t="s">
+      <c r="D9" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="4"/>
+      <c r="B10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" s="4"/>
+      <c r="B11" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" s="5"/>
+      <c r="B12" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" s="6" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" t="s">
+      <c r="B13" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" s="8"/>
+      <c r="B14" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" s="8"/>
+      <c r="B15" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C15" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="D9" t="s">
-        <v>34</v>
-      </c>
-      <c r="F9" t="s">
-        <v>32</v>
-      </c>
-      <c r="G9" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B10" t="s">
-        <v>39</v>
-      </c>
-      <c r="C10" t="s">
+      <c r="D15" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" s="8"/>
+      <c r="B16" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C16" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D10" t="s">
-        <v>40</v>
-      </c>
-      <c r="F10" t="s">
-        <v>41</v>
-      </c>
-      <c r="G10" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B11" t="s">
-        <v>36</v>
-      </c>
-      <c r="C11" t="s">
+      <c r="D16" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" s="8"/>
+      <c r="B17" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C17" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="D11" t="s">
-        <v>38</v>
-      </c>
-      <c r="F11" t="s">
-        <v>32</v>
-      </c>
-      <c r="G11" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B12" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" t="s">
+      <c r="D17" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" s="8"/>
+      <c r="B18" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D12" t="s">
-        <v>34</v>
-      </c>
-      <c r="F12" t="s">
-        <v>17</v>
-      </c>
-      <c r="G12" t="s">
-        <v>20</v>
-      </c>
+      <c r="D18" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" s="8"/>
+      <c r="B19" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="H19" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" s="9"/>
+      <c r="B20" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A2:A12"/>
+    <mergeCell ref="A13:A20"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>

</xml_diff>